<commit_message>
combined FULL dataset issues with lmer model - variations using 1/Site or 1/Transect
</commit_message>
<xml_diff>
--- a/raw/Labbook.xlsx
+++ b/raw/Labbook.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/snekz/Desktop/Thesis/Rawdata/ABSsecondround/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/snekz/Desktop/Thesis/ABS_second_round/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57D7AA44-B1F9-414C-9B1A-8ED0D4B2D5D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04577D3D-1F64-EF41-9D25-D7F9A2332BB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9820" yWindow="760" windowWidth="20420" windowHeight="18880" activeTab="2" xr2:uid="{E68C0344-DB4F-8849-856A-D4D7A651933D}"/>
+    <workbookView xWindow="9820" yWindow="760" windowWidth="20420" windowHeight="18880" activeTab="3" xr2:uid="{E68C0344-DB4F-8849-856A-D4D7A651933D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1314" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1316" uniqueCount="98">
   <si>
     <t>Harvest date</t>
   </si>
@@ -332,6 +332,9 @@
   </si>
   <si>
     <t>total_W</t>
+  </si>
+  <si>
+    <t>New_tube</t>
   </si>
 </sst>
 </file>
@@ -935,7 +938,7 @@
   <dimension ref="A1:K145"/>
   <sheetViews>
     <sheetView zoomScale="85" workbookViewId="0">
-      <selection activeCell="K54" sqref="K54"/>
+      <selection activeCell="I2" sqref="I2:I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5044,6 +5047,73 @@
     </row>
   </sheetData>
   <mergeCells count="76">
+    <mergeCell ref="I144:I145"/>
+    <mergeCell ref="I134:I135"/>
+    <mergeCell ref="I136:I137"/>
+    <mergeCell ref="I138:I139"/>
+    <mergeCell ref="I140:I141"/>
+    <mergeCell ref="I142:I143"/>
+    <mergeCell ref="I124:I125"/>
+    <mergeCell ref="I126:I127"/>
+    <mergeCell ref="I128:I129"/>
+    <mergeCell ref="I130:I131"/>
+    <mergeCell ref="I132:I133"/>
+    <mergeCell ref="I114:I115"/>
+    <mergeCell ref="I116:I117"/>
+    <mergeCell ref="I118:I119"/>
+    <mergeCell ref="I120:I121"/>
+    <mergeCell ref="I122:I123"/>
+    <mergeCell ref="I104:I105"/>
+    <mergeCell ref="I106:I107"/>
+    <mergeCell ref="I108:I109"/>
+    <mergeCell ref="I110:I111"/>
+    <mergeCell ref="I112:I113"/>
+    <mergeCell ref="I94:I95"/>
+    <mergeCell ref="I96:I97"/>
+    <mergeCell ref="I98:I99"/>
+    <mergeCell ref="I100:I101"/>
+    <mergeCell ref="I102:I103"/>
+    <mergeCell ref="I84:I85"/>
+    <mergeCell ref="I86:I87"/>
+    <mergeCell ref="I88:I89"/>
+    <mergeCell ref="I90:I91"/>
+    <mergeCell ref="I92:I93"/>
+    <mergeCell ref="I74:I75"/>
+    <mergeCell ref="I76:I77"/>
+    <mergeCell ref="I78:I79"/>
+    <mergeCell ref="I80:I81"/>
+    <mergeCell ref="I82:I83"/>
+    <mergeCell ref="I22:I23"/>
+    <mergeCell ref="I24:I25"/>
+    <mergeCell ref="I12:I13"/>
+    <mergeCell ref="I16:I17"/>
+    <mergeCell ref="I18:I19"/>
+    <mergeCell ref="I20:I21"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="I4:I5"/>
+    <mergeCell ref="I6:I7"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="I10:I11"/>
+    <mergeCell ref="A122:A145"/>
+    <mergeCell ref="A2:A25"/>
+    <mergeCell ref="A26:A49"/>
+    <mergeCell ref="A50:A73"/>
+    <mergeCell ref="A74:A97"/>
+    <mergeCell ref="A98:A121"/>
+    <mergeCell ref="I36:I37"/>
+    <mergeCell ref="I40:I41"/>
+    <mergeCell ref="I42:I43"/>
+    <mergeCell ref="I44:I45"/>
+    <mergeCell ref="I26:I27"/>
+    <mergeCell ref="I28:I29"/>
+    <mergeCell ref="I30:I31"/>
+    <mergeCell ref="I32:I33"/>
+    <mergeCell ref="I34:I35"/>
+    <mergeCell ref="I46:I47"/>
+    <mergeCell ref="I48:I49"/>
+    <mergeCell ref="I50:I51"/>
+    <mergeCell ref="I52:I53"/>
+    <mergeCell ref="I54:I55"/>
     <mergeCell ref="I66:I67"/>
     <mergeCell ref="I68:I69"/>
     <mergeCell ref="I70:I71"/>
@@ -5053,73 +5123,6 @@
     <mergeCell ref="I60:I61"/>
     <mergeCell ref="I62:I63"/>
     <mergeCell ref="I64:I65"/>
-    <mergeCell ref="I46:I47"/>
-    <mergeCell ref="I48:I49"/>
-    <mergeCell ref="I50:I51"/>
-    <mergeCell ref="I52:I53"/>
-    <mergeCell ref="I54:I55"/>
-    <mergeCell ref="I36:I37"/>
-    <mergeCell ref="I40:I41"/>
-    <mergeCell ref="I42:I43"/>
-    <mergeCell ref="I44:I45"/>
-    <mergeCell ref="I26:I27"/>
-    <mergeCell ref="I28:I29"/>
-    <mergeCell ref="I30:I31"/>
-    <mergeCell ref="I32:I33"/>
-    <mergeCell ref="I34:I35"/>
-    <mergeCell ref="A122:A145"/>
-    <mergeCell ref="A2:A25"/>
-    <mergeCell ref="A26:A49"/>
-    <mergeCell ref="A50:A73"/>
-    <mergeCell ref="A74:A97"/>
-    <mergeCell ref="A98:A121"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="I4:I5"/>
-    <mergeCell ref="I6:I7"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="I10:I11"/>
-    <mergeCell ref="I22:I23"/>
-    <mergeCell ref="I24:I25"/>
-    <mergeCell ref="I12:I13"/>
-    <mergeCell ref="I16:I17"/>
-    <mergeCell ref="I18:I19"/>
-    <mergeCell ref="I20:I21"/>
-    <mergeCell ref="I74:I75"/>
-    <mergeCell ref="I76:I77"/>
-    <mergeCell ref="I78:I79"/>
-    <mergeCell ref="I80:I81"/>
-    <mergeCell ref="I82:I83"/>
-    <mergeCell ref="I84:I85"/>
-    <mergeCell ref="I86:I87"/>
-    <mergeCell ref="I88:I89"/>
-    <mergeCell ref="I90:I91"/>
-    <mergeCell ref="I92:I93"/>
-    <mergeCell ref="I94:I95"/>
-    <mergeCell ref="I96:I97"/>
-    <mergeCell ref="I98:I99"/>
-    <mergeCell ref="I100:I101"/>
-    <mergeCell ref="I102:I103"/>
-    <mergeCell ref="I104:I105"/>
-    <mergeCell ref="I106:I107"/>
-    <mergeCell ref="I108:I109"/>
-    <mergeCell ref="I110:I111"/>
-    <mergeCell ref="I112:I113"/>
-    <mergeCell ref="I114:I115"/>
-    <mergeCell ref="I116:I117"/>
-    <mergeCell ref="I118:I119"/>
-    <mergeCell ref="I120:I121"/>
-    <mergeCell ref="I122:I123"/>
-    <mergeCell ref="I124:I125"/>
-    <mergeCell ref="I126:I127"/>
-    <mergeCell ref="I128:I129"/>
-    <mergeCell ref="I130:I131"/>
-    <mergeCell ref="I132:I133"/>
-    <mergeCell ref="I144:I145"/>
-    <mergeCell ref="I134:I135"/>
-    <mergeCell ref="I136:I137"/>
-    <mergeCell ref="I138:I139"/>
-    <mergeCell ref="I140:I141"/>
-    <mergeCell ref="I142:I143"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8046,7 +8049,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36E71E6A-D131-9C45-A84B-AB9D69CAB7F3}">
   <dimension ref="B1:H25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
@@ -8523,8 +8526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B42BF2A1-BEFF-8840-AF7D-96943EA92104}">
   <dimension ref="A1:D73"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8539,6 +8542,12 @@
       <c r="B1" t="s">
         <v>53</v>
       </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
@@ -9250,6 +9259,18 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="D35:D37"/>
+    <mergeCell ref="D2:D4"/>
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="D11:D13"/>
+    <mergeCell ref="D14:D16"/>
+    <mergeCell ref="D17:D19"/>
+    <mergeCell ref="D20:D22"/>
+    <mergeCell ref="D23:D25"/>
+    <mergeCell ref="D26:D28"/>
+    <mergeCell ref="D29:D31"/>
+    <mergeCell ref="D32:D34"/>
     <mergeCell ref="D71:D73"/>
     <mergeCell ref="D38:D40"/>
     <mergeCell ref="D41:D43"/>
@@ -9262,18 +9283,6 @@
     <mergeCell ref="D62:D64"/>
     <mergeCell ref="D65:D67"/>
     <mergeCell ref="D68:D70"/>
-    <mergeCell ref="D35:D37"/>
-    <mergeCell ref="D2:D4"/>
-    <mergeCell ref="D5:D7"/>
-    <mergeCell ref="D8:D10"/>
-    <mergeCell ref="D11:D13"/>
-    <mergeCell ref="D14:D16"/>
-    <mergeCell ref="D17:D19"/>
-    <mergeCell ref="D20:D22"/>
-    <mergeCell ref="D23:D25"/>
-    <mergeCell ref="D26:D28"/>
-    <mergeCell ref="D29:D31"/>
-    <mergeCell ref="D32:D34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>